<commit_message>
Updated XPS plotting to python file
</commit_message>
<xml_diff>
--- a/06_XPS_Analysis/data/raw/BTY_H2O.xlsx
+++ b/06_XPS_Analysis/data/raw/BTY_H2O.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dreec\PycharmProjects\Paper2\06_XPS_Analysis\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2615043-1226-4745-B368-012CC853E5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAC3FB4F-0A4D-4B9D-B892-F22CEF4F3D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{2FDC9F2C-36C8-484B-A712-7BA5BBFF01BC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{26604027-7031-42ED-B2E0-9A5FB7467941}"/>
   </bookViews>
   <sheets>
     <sheet name="BTY_H2O" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -934,16 +934,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3661B4EA-8462-4B8B-AAC5-F435D81CDB63}">
-  <dimension ref="A1:W248"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B100C3E-11C0-4E16-8ADB-50C1E2C3AB3E}">
+  <dimension ref="A1:X248"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -980,8 +978,11 @@
       <c r="U1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="V1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1016,10 +1017,13 @@
         <v>4</v>
       </c>
       <c r="U2">
-        <v>74.709999999999994</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+        <v>74.58</v>
+      </c>
+      <c r="V2">
+        <v>75.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1054,10 +1058,13 @@
         <v>5</v>
       </c>
       <c r="U3">
-        <v>1.84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+        <v>1.65</v>
+      </c>
+      <c r="V3">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1092,10 +1099,13 @@
         <v>6</v>
       </c>
       <c r="U4">
-        <v>6591.62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+        <v>5362.59</v>
+      </c>
+      <c r="V4">
+        <v>1228.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1132,8 +1142,11 @@
       <c r="U5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="V5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1192,13 +1205,16 @@
         <v>17</v>
       </c>
       <c r="V7" t="s">
+        <v>17</v>
+      </c>
+      <c r="W7" t="s">
         <v>12</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>544.96</v>
       </c>
@@ -1262,8 +1278,11 @@
       <c r="W8" s="1">
         <v>350.92129999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X8" s="1">
+        <v>350.92129999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>544.86</v>
       </c>
@@ -1327,8 +1346,11 @@
       <c r="W9" s="1">
         <v>318.67669999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X9" s="1">
+        <v>318.67669999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>544.76</v>
       </c>
@@ -1392,8 +1414,11 @@
       <c r="W10" s="1">
         <v>322.44560000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X10" s="1">
+        <v>322.44560000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>544.66</v>
       </c>
@@ -1457,8 +1482,11 @@
       <c r="W11" s="1">
         <v>335.4271</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X11" s="1">
+        <v>335.4271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>544.55999999999995</v>
       </c>
@@ -1522,8 +1550,11 @@
       <c r="W12" s="1">
         <v>340.87099999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X12" s="1">
+        <v>340.87099999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>544.46</v>
       </c>
@@ -1587,8 +1618,11 @@
       <c r="W13" s="1">
         <v>331.6583</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X13" s="1">
+        <v>331.6583</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>544.36</v>
       </c>
@@ -1652,8 +1686,11 @@
       <c r="W14" s="1">
         <v>329.98320000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X14" s="1">
+        <v>329.98320000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>544.26</v>
       </c>
@@ -1717,8 +1754,11 @@
       <c r="W15" s="1">
         <v>341.70850000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X15" s="1">
+        <v>341.70850000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>544.16</v>
       </c>
@@ -1782,8 +1822,11 @@
       <c r="W16" s="1">
         <v>319.51420000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X16" s="1">
+        <v>319.51420000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>544.05999999999995</v>
       </c>
@@ -1847,8 +1890,11 @@
       <c r="W17" s="1">
         <v>298.995</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X17" s="1">
+        <v>298.995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>543.96</v>
       </c>
@@ -1912,8 +1958,11 @@
       <c r="W18" s="1">
         <v>315.74540000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X18" s="1">
+        <v>315.74540000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>543.86</v>
       </c>
@@ -1977,8 +2026,11 @@
       <c r="W19" s="1">
         <v>309.464</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X19" s="1">
+        <v>309.464</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>543.76</v>
       </c>
@@ -2042,8 +2094,11 @@
       <c r="W20" s="1">
         <v>295.64490000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X20" s="1">
+        <v>295.64490000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>543.66</v>
       </c>
@@ -2107,8 +2162,11 @@
       <c r="W21" s="1">
         <v>305.69510000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X21" s="1">
+        <v>305.69510000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>543.55999999999995</v>
       </c>
@@ -2172,8 +2230,11 @@
       <c r="W22" s="1">
         <v>304.43889999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X22" s="1">
+        <v>304.43889999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>543.46</v>
       </c>
@@ -2237,8 +2298,11 @@
       <c r="W23" s="1">
         <v>314.90789999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X23" s="1">
+        <v>314.90789999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>543.36</v>
       </c>
@@ -2302,8 +2366,11 @@
       <c r="W24" s="1">
         <v>285.17590000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X24" s="1">
+        <v>285.17590000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>543.26</v>
       </c>
@@ -2367,8 +2434,11 @@
       <c r="W25" s="1">
         <v>289.78219999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X25" s="1">
+        <v>289.78219999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>543.16</v>
       </c>
@@ -2432,8 +2502,11 @@
       <c r="W26" s="1">
         <v>295.64490000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X26" s="1">
+        <v>295.64490000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>543.05999999999995</v>
       </c>
@@ -2497,8 +2570,11 @@
       <c r="W27" s="1">
         <v>291.87599999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X27" s="1">
+        <v>291.87599999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>542.96</v>
       </c>
@@ -2562,8 +2638,11 @@
       <c r="W28" s="1">
         <v>292.29480000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X28" s="1">
+        <v>292.29480000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>542.86</v>
       </c>
@@ -2627,8 +2706,11 @@
       <c r="W29" s="1">
         <v>289.78219999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X29" s="1">
+        <v>289.78219999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>542.76</v>
       </c>
@@ -2692,8 +2774,11 @@
       <c r="W30" s="1">
         <v>280.56950000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X30" s="1">
+        <v>280.56950000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>542.66</v>
       </c>
@@ -2757,8 +2842,11 @@
       <c r="W31" s="1">
         <v>282.66329999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X31" s="1">
+        <v>282.66329999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>542.55999999999995</v>
       </c>
@@ -2822,8 +2910,11 @@
       <c r="W32" s="1">
         <v>277.63819999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X32" s="1">
+        <v>277.63819999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>542.46</v>
       </c>
@@ -2887,8 +2978,11 @@
       <c r="W33" s="1">
         <v>286.43220000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X33" s="1">
+        <v>286.43220000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>542.36</v>
       </c>
@@ -2952,8 +3046,11 @@
       <c r="W34" s="1">
         <v>279.73200000000003</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X34" s="1">
+        <v>279.73200000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>542.26</v>
       </c>
@@ -3017,8 +3114,11 @@
       <c r="W35" s="1">
         <v>268.00670000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X35" s="1">
+        <v>268.00670000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>542.16</v>
       </c>
@@ -3082,8 +3182,11 @@
       <c r="W36" s="1">
         <v>269.68169999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X36" s="1">
+        <v>269.68169999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>542.05999999999995</v>
       </c>
@@ -3147,8 +3250,11 @@
       <c r="W37" s="1">
         <v>249.5812</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X37" s="1">
+        <v>249.5812</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>541.96</v>
       </c>
@@ -3212,8 +3318,11 @@
       <c r="W38" s="1">
         <v>272.1943</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X38" s="1">
+        <v>272.1943</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>541.86</v>
       </c>
@@ -3277,8 +3386,11 @@
       <c r="W39" s="1">
         <v>275.9631</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X39" s="1">
+        <v>275.9631</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>541.76</v>
       </c>
@@ -3342,8 +3454,11 @@
       <c r="W40" s="1">
         <v>253.7688</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X40" s="1">
+        <v>253.7688</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>541.66</v>
       </c>
@@ -3407,8 +3522,11 @@
       <c r="W41" s="1">
         <v>271.35680000000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X41" s="1">
+        <v>271.35680000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>541.55999999999995</v>
       </c>
@@ -3472,8 +3590,11 @@
       <c r="W42" s="1">
         <v>247.90620000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X42" s="1">
+        <v>247.90620000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>541.46</v>
       </c>
@@ -3537,8 +3658,11 @@
       <c r="W43" s="1">
         <v>269.26299999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X43" s="1">
+        <v>269.26299999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>541.36</v>
       </c>
@@ -3602,8 +3726,11 @@
       <c r="W44" s="1">
         <v>253.7688</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X44" s="1">
+        <v>253.7688</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>541.26</v>
       </c>
@@ -3667,8 +3794,11 @@
       <c r="W45" s="1">
         <v>250.4188</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X45" s="1">
+        <v>250.4188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>541.16</v>
       </c>
@@ -3732,8 +3862,11 @@
       <c r="W46" s="1">
         <v>239.94970000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X46" s="1">
+        <v>239.94970000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>541.05999999999995</v>
       </c>
@@ -3797,8 +3930,11 @@
       <c r="W47" s="1">
         <v>229.89949999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X47" s="1">
+        <v>229.89949999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>540.96</v>
       </c>
@@ -3862,8 +3998,11 @@
       <c r="W48" s="1">
         <v>249.5812</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X48" s="1">
+        <v>249.5812</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>540.86</v>
       </c>
@@ -3927,8 +4066,11 @@
       <c r="W49" s="1">
         <v>256.7002</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X49" s="1">
+        <v>256.7002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>540.76</v>
       </c>
@@ -3992,8 +4134,11 @@
       <c r="W50" s="1">
         <v>250.83750000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X50" s="1">
+        <v>250.83750000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>540.66</v>
       </c>
@@ -4057,8 +4202,11 @@
       <c r="W51" s="1">
         <v>243.2998</v>
       </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X51" s="1">
+        <v>243.2998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>540.55999999999995</v>
       </c>
@@ -4122,8 +4270,11 @@
       <c r="W52" s="1">
         <v>234.9246</v>
       </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X52" s="1">
+        <v>234.9246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>540.46</v>
       </c>
@@ -4187,8 +4338,11 @@
       <c r="W53" s="1">
         <v>233.24959999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X53" s="1">
+        <v>233.24959999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>540.36</v>
       </c>
@@ -4252,8 +4406,11 @@
       <c r="W54" s="1">
         <v>246.6499</v>
       </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X54" s="1">
+        <v>246.6499</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>540.26</v>
       </c>
@@ -4317,8 +4474,11 @@
       <c r="W55" s="1">
         <v>233.66829999999999</v>
       </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X55" s="1">
+        <v>233.66829999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>540.16</v>
       </c>
@@ -4382,8 +4542,11 @@
       <c r="W56" s="1">
         <v>219.8492</v>
       </c>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X56" s="1">
+        <v>219.8492</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>540.05999999999995</v>
       </c>
@@ -4447,8 +4610,11 @@
       <c r="W57" s="1">
         <v>219.8492</v>
       </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X57" s="1">
+        <v>219.8492</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>539.96</v>
       </c>
@@ -4512,8 +4678,11 @@
       <c r="W58" s="1">
         <v>229.89949999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X58" s="1">
+        <v>229.89949999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>539.86</v>
       </c>
@@ -4577,8 +4746,11 @@
       <c r="W59" s="1">
         <v>218.59299999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X59" s="1">
+        <v>218.59299999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>539.76</v>
       </c>
@@ -4642,8 +4814,11 @@
       <c r="W60" s="1">
         <v>208.124</v>
       </c>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X60" s="1">
+        <v>208.124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>539.66</v>
       </c>
@@ -4707,8 +4882,11 @@
       <c r="W61" s="1">
         <v>223.6181</v>
       </c>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X61" s="1">
+        <v>223.6181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>539.55999999999995</v>
       </c>
@@ -4772,8 +4950,11 @@
       <c r="W62" s="1">
         <v>224.0369</v>
       </c>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X62" s="1">
+        <v>224.0369</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>539.46</v>
       </c>
@@ -4837,8 +5018,11 @@
       <c r="W63" s="1">
         <v>215.66159999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X63" s="1">
+        <v>215.66159999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>539.36</v>
       </c>
@@ -4902,8 +5086,11 @@
       <c r="W64" s="1">
         <v>204.35509999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X64" s="1">
+        <v>204.35509999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>539.26</v>
       </c>
@@ -4967,8 +5154,11 @@
       <c r="W65" s="1">
         <v>198.0737</v>
       </c>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X65" s="1">
+        <v>198.0737</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>539.16</v>
       </c>
@@ -5032,8 +5222,11 @@
       <c r="W66" s="1">
         <v>213.98660000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X66" s="1">
+        <v>213.98660000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>539.05999999999995</v>
       </c>
@@ -5097,8 +5290,11 @@
       <c r="W67" s="1">
         <v>213.1491</v>
       </c>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X67" s="1">
+        <v>213.1491</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>538.96</v>
       </c>
@@ -5162,8 +5358,11 @@
       <c r="W68" s="1">
         <v>192.21109999999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X68" s="1">
+        <v>192.21109999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>538.86</v>
       </c>
@@ -5227,8 +5426,11 @@
       <c r="W69" s="1">
         <v>195.97989999999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X69" s="1">
+        <v>195.97989999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>538.76</v>
       </c>
@@ -5292,8 +5494,11 @@
       <c r="W70" s="1">
         <v>195.14240000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X70" s="1">
+        <v>195.14240000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>538.66</v>
       </c>
@@ -5357,8 +5562,11 @@
       <c r="W71" s="1">
         <v>192.62979999999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X71" s="1">
+        <v>192.62979999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>538.55999999999995</v>
       </c>
@@ -5422,8 +5630,11 @@
       <c r="W72" s="1">
         <v>200.16749999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X72" s="1">
+        <v>200.16749999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>538.46</v>
       </c>
@@ -5487,8 +5698,11 @@
       <c r="W73" s="1">
         <v>197.2362</v>
       </c>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X73" s="1">
+        <v>197.2362</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>538.36</v>
       </c>
@@ -5552,8 +5766,11 @@
       <c r="W74" s="1">
         <v>197.2362</v>
       </c>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X74" s="1">
+        <v>197.2362</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>538.26</v>
       </c>
@@ -5617,8 +5834,11 @@
       <c r="W75" s="1">
         <v>211.89279999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X75" s="1">
+        <v>211.89279999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>538.16</v>
       </c>
@@ -5682,8 +5902,11 @@
       <c r="W76" s="1">
         <v>184.67339999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X76" s="1">
+        <v>184.67339999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>538.05999999999995</v>
       </c>
@@ -5747,8 +5970,11 @@
       <c r="W77" s="1">
         <v>184.25460000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X77" s="1">
+        <v>184.25460000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>537.96</v>
       </c>
@@ -5812,8 +6038,11 @@
       <c r="W78" s="1">
         <v>175.0419</v>
       </c>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X78" s="1">
+        <v>175.0419</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>537.86</v>
       </c>
@@ -5877,8 +6106,11 @@
       <c r="W79" s="1">
         <v>186.3484</v>
       </c>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X79" s="1">
+        <v>186.3484</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>537.76</v>
       </c>
@@ -5942,8 +6174,11 @@
       <c r="W80" s="1">
         <v>196.81739999999999</v>
       </c>
-    </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X80" s="1">
+        <v>196.81739999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>537.66</v>
       </c>
@@ -6007,8 +6242,11 @@
       <c r="W81" s="1">
         <v>186.3484</v>
       </c>
-    </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X81" s="1">
+        <v>186.3484</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>537.55999999999995</v>
       </c>
@@ -6072,8 +6310,11 @@
       <c r="W82" s="1">
         <v>187.60470000000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X82" s="1">
+        <v>187.60470000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>537.46</v>
       </c>
@@ -6137,8 +6378,11 @@
       <c r="W83" s="1">
         <v>177.97319999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X83" s="1">
+        <v>177.97319999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>537.36</v>
       </c>
@@ -6202,8 +6446,11 @@
       <c r="W84" s="1">
         <v>190.1173</v>
       </c>
-    </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X84" s="1">
+        <v>190.1173</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>537.26</v>
       </c>
@@ -6267,8 +6514,11 @@
       <c r="W85" s="1">
         <v>180.48580000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X85" s="1">
+        <v>180.48580000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>537.16</v>
       </c>
@@ -6332,8 +6582,11 @@
       <c r="W86" s="1">
         <v>170.01679999999999</v>
       </c>
-    </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X86" s="1">
+        <v>170.01679999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>537.05999999999995</v>
       </c>
@@ -6389,16 +6642,19 @@
         <v>177.55439999999999</v>
       </c>
       <c r="U87" s="1">
+        <v>177.55439999999999</v>
+      </c>
+      <c r="V87" s="1">
         <v>177.55449999999999</v>
       </c>
-      <c r="V87" s="1">
+      <c r="W87" s="1">
         <v>177.55439999999999</v>
       </c>
-      <c r="W87" s="1">
+      <c r="X87" s="1">
         <v>177.55449999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>536.96</v>
       </c>
@@ -6454,16 +6710,19 @@
         <v>177.55439999999999</v>
       </c>
       <c r="U88" s="1">
+        <v>177.55439999999999</v>
+      </c>
+      <c r="V88" s="1">
         <v>177.55459999999999</v>
       </c>
-      <c r="V88" s="1">
+      <c r="W88" s="1">
         <v>177.55439999999999</v>
       </c>
-      <c r="W88" s="1">
+      <c r="X88" s="1">
         <v>177.55459999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>536.86</v>
       </c>
@@ -6519,16 +6778,19 @@
         <v>166.24789999999999</v>
       </c>
       <c r="U89" s="1">
+        <v>166.24789999999999</v>
+      </c>
+      <c r="V89" s="1">
         <v>166.2482</v>
       </c>
-      <c r="V89" s="1">
+      <c r="W89" s="1">
         <v>166.24789999999999</v>
       </c>
-      <c r="W89" s="1">
+      <c r="X89" s="1">
         <v>166.2482</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>536.76</v>
       </c>
@@ -6584,16 +6846,19 @@
         <v>175.8794</v>
       </c>
       <c r="U90" s="1">
+        <v>175.8794</v>
+      </c>
+      <c r="V90" s="1">
         <v>175.87989999999999</v>
       </c>
-      <c r="V90" s="1">
+      <c r="W90" s="1">
         <v>175.8794</v>
       </c>
-      <c r="W90" s="1">
+      <c r="X90" s="1">
         <v>175.87989999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>536.66</v>
       </c>
@@ -6649,16 +6914,19 @@
         <v>179.6482</v>
       </c>
       <c r="U91" s="1">
+        <v>179.64830000000001</v>
+      </c>
+      <c r="V91" s="1">
         <v>179.6491</v>
       </c>
-      <c r="V91" s="1">
+      <c r="W91" s="1">
         <v>179.6482</v>
       </c>
-      <c r="W91" s="1">
-        <v>179.6491</v>
-      </c>
-    </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X91" s="1">
+        <v>179.64920000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>536.55999999999995</v>
       </c>
@@ -6714,16 +6982,19 @@
         <v>185.09209999999999</v>
       </c>
       <c r="U92" s="1">
-        <v>185.09360000000001</v>
+        <v>185.09219999999999</v>
       </c>
       <c r="V92" s="1">
+        <v>185.09379999999999</v>
+      </c>
+      <c r="W92" s="1">
         <v>185.09209999999999</v>
       </c>
-      <c r="W92" s="1">
-        <v>185.09360000000001</v>
-      </c>
-    </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X92" s="1">
+        <v>185.09379999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>536.46</v>
       </c>
@@ -6779,16 +7050,19 @@
         <v>187.1859</v>
       </c>
       <c r="U93" s="1">
-        <v>187.1884</v>
+        <v>187.18600000000001</v>
       </c>
       <c r="V93" s="1">
+        <v>187.18879999999999</v>
+      </c>
+      <c r="W93" s="1">
         <v>187.1859</v>
       </c>
-      <c r="W93" s="1">
-        <v>187.1884</v>
-      </c>
-    </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X93" s="1">
+        <v>187.18889999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>536.36</v>
       </c>
@@ -6844,16 +7118,19 @@
         <v>197.2362</v>
       </c>
       <c r="U94" s="1">
-        <v>197.2405</v>
+        <v>197.2363</v>
       </c>
       <c r="V94" s="1">
+        <v>197.24119999999999</v>
+      </c>
+      <c r="W94" s="1">
         <v>197.2362</v>
       </c>
-      <c r="W94" s="1">
-        <v>197.2405</v>
-      </c>
-    </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X94" s="1">
+        <v>197.2413</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>536.26</v>
       </c>
@@ -6909,16 +7186,19 @@
         <v>188.86099999999999</v>
       </c>
       <c r="U95" s="1">
-        <v>188.8682</v>
+        <v>188.86109999999999</v>
       </c>
       <c r="V95" s="1">
+        <v>188.86969999999999</v>
+      </c>
+      <c r="W95" s="1">
         <v>188.86099999999999</v>
       </c>
-      <c r="W95" s="1">
-        <v>188.8682</v>
-      </c>
-    </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X95" s="1">
+        <v>188.8698</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>536.16</v>
       </c>
@@ -6974,16 +7254,19 @@
         <v>185.09209999999999</v>
       </c>
       <c r="U96" s="1">
-        <v>185.10419999999999</v>
+        <v>185.0925</v>
       </c>
       <c r="V96" s="1">
+        <v>185.107</v>
+      </c>
+      <c r="W96" s="1">
         <v>185.09209999999999</v>
       </c>
-      <c r="W96" s="1">
-        <v>185.10419999999999</v>
-      </c>
-    </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X96" s="1">
+        <v>185.10740000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>536.05999999999995</v>
       </c>
@@ -7039,16 +7322,19 @@
         <v>182.9983</v>
       </c>
       <c r="U97" s="1">
-        <v>183.01840000000001</v>
+        <v>182.99889999999999</v>
       </c>
       <c r="V97" s="1">
+        <v>183.02340000000001</v>
+      </c>
+      <c r="W97" s="1">
         <v>182.9983</v>
       </c>
-      <c r="W97" s="1">
-        <v>183.01840000000001</v>
-      </c>
-    </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X97" s="1">
+        <v>183.024</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>535.96</v>
       </c>
@@ -7104,16 +7390,19 @@
         <v>188.86099999999999</v>
       </c>
       <c r="U98" s="1">
-        <v>188.8939</v>
+        <v>188.8621</v>
       </c>
       <c r="V98" s="1">
+        <v>188.90260000000001</v>
+      </c>
+      <c r="W98" s="1">
         <v>188.86099999999999</v>
       </c>
-      <c r="W98" s="1">
-        <v>188.8939</v>
-      </c>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X98" s="1">
+        <v>188.90379999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>535.86</v>
       </c>
@@ -7169,16 +7458,19 @@
         <v>191.37350000000001</v>
       </c>
       <c r="U99" s="1">
-        <v>191.4273</v>
+        <v>191.37569999999999</v>
       </c>
       <c r="V99" s="1">
+        <v>191.44220000000001</v>
+      </c>
+      <c r="W99" s="1">
         <v>191.37350000000001</v>
       </c>
-      <c r="W99" s="1">
-        <v>191.4273</v>
-      </c>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X99" s="1">
+        <v>191.4444</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>535.76</v>
       </c>
@@ -7234,16 +7526,19 @@
         <v>179.2295</v>
       </c>
       <c r="U100" s="1">
-        <v>179.31610000000001</v>
+        <v>179.23339999999999</v>
       </c>
       <c r="V100" s="1">
+        <v>179.3409</v>
+      </c>
+      <c r="W100" s="1">
         <v>179.2295</v>
       </c>
-      <c r="W100" s="1">
-        <v>179.31610000000001</v>
-      </c>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X100" s="1">
+        <v>179.34479999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>535.66</v>
       </c>
@@ -7299,16 +7594,19 @@
         <v>177.97319999999999</v>
       </c>
       <c r="U101" s="1">
-        <v>178.1114</v>
+        <v>177.98009999999999</v>
       </c>
       <c r="V101" s="1">
+        <v>178.15180000000001</v>
+      </c>
+      <c r="W101" s="1">
         <v>177.97319999999999</v>
       </c>
-      <c r="W101" s="1">
-        <v>178.1114</v>
-      </c>
-    </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X101" s="1">
+        <v>178.15870000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>535.55999999999995</v>
       </c>
@@ -7364,16 +7662,19 @@
         <v>186.3484</v>
       </c>
       <c r="U102" s="1">
-        <v>186.56659999999999</v>
+        <v>186.36070000000001</v>
       </c>
       <c r="V102" s="1">
+        <v>186.63239999999999</v>
+      </c>
+      <c r="W102" s="1">
         <v>186.3484</v>
       </c>
-      <c r="W102" s="1">
-        <v>186.56659999999999</v>
-      </c>
-    </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X102" s="1">
+        <v>186.6447</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>535.46</v>
       </c>
@@ -7429,16 +7730,19 @@
         <v>188.86099999999999</v>
       </c>
       <c r="U103" s="1">
-        <v>186.6326</v>
+        <v>186.31309999999999</v>
       </c>
       <c r="V103" s="1">
+        <v>186.73609999999999</v>
+      </c>
+      <c r="W103" s="1">
         <v>186.29159999999999</v>
       </c>
-      <c r="W103" s="1">
-        <v>186.6326</v>
-      </c>
-    </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X103" s="1">
+        <v>186.7576</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>535.36</v>
       </c>
@@ -7494,16 +7798,19 @@
         <v>204.35509999999999</v>
       </c>
       <c r="U104" s="1">
-        <v>186.7621</v>
+        <v>186.27170000000001</v>
       </c>
       <c r="V104" s="1">
+        <v>186.9213</v>
+      </c>
+      <c r="W104" s="1">
         <v>186.2347</v>
       </c>
-      <c r="W104" s="1">
-        <v>186.7621</v>
-      </c>
-    </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X104" s="1">
+        <v>186.95840000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>535.26</v>
       </c>
@@ -7559,16 +7866,19 @@
         <v>191.79230000000001</v>
       </c>
       <c r="U105" s="1">
-        <v>186.9854</v>
+        <v>186.24109999999999</v>
       </c>
       <c r="V105" s="1">
+        <v>187.23050000000001</v>
+      </c>
+      <c r="W105" s="1">
         <v>186.17760000000001</v>
       </c>
-      <c r="W105" s="1">
-        <v>186.9854</v>
-      </c>
-    </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X105" s="1">
+        <v>187.29400000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>535.16</v>
       </c>
@@ -7624,16 +7934,19 @@
         <v>201.4238</v>
       </c>
       <c r="U106" s="1">
-        <v>187.3451</v>
+        <v>186.22739999999999</v>
       </c>
       <c r="V106" s="1">
+        <v>187.71010000000001</v>
+      </c>
+      <c r="W106" s="1">
         <v>186.12039999999999</v>
       </c>
-      <c r="W106" s="1">
-        <v>187.3451</v>
-      </c>
-    </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X106" s="1">
+        <v>187.81710000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>535.05999999999995</v>
       </c>
@@ -7689,16 +8002,19 @@
         <v>202.68010000000001</v>
       </c>
       <c r="U107" s="1">
-        <v>187.90129999999999</v>
+        <v>186.2406</v>
       </c>
       <c r="V107" s="1">
+        <v>188.43090000000001</v>
+      </c>
+      <c r="W107" s="1">
         <v>186.06309999999999</v>
       </c>
-      <c r="W107" s="1">
-        <v>187.90129999999999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X107" s="1">
+        <v>188.60839999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>534.96</v>
       </c>
@@ -7754,16 +8070,19 @@
         <v>198.0737</v>
       </c>
       <c r="U108" s="1">
-        <v>188.74100000000001</v>
+        <v>186.29900000000001</v>
       </c>
       <c r="V108" s="1">
+        <v>189.50620000000001</v>
+      </c>
+      <c r="W108" s="1">
         <v>186.00559999999999</v>
       </c>
-      <c r="W108" s="1">
-        <v>188.74100000000001</v>
-      </c>
-    </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X108" s="1">
+        <v>189.7997</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>534.86</v>
       </c>
@@ -7819,16 +8138,19 @@
         <v>188.86099999999999</v>
       </c>
       <c r="U109" s="1">
-        <v>189.9846</v>
+        <v>186.42490000000001</v>
       </c>
       <c r="V109" s="1">
+        <v>191.04650000000001</v>
+      </c>
+      <c r="W109" s="1">
         <v>185.94800000000001</v>
       </c>
-      <c r="W109" s="1">
-        <v>189.9846</v>
-      </c>
-    </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X109" s="1">
+        <v>191.52340000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>534.76</v>
       </c>
@@ -7884,16 +8206,19 @@
         <v>207.28639999999999</v>
       </c>
       <c r="U110" s="1">
-        <v>191.78620000000001</v>
+        <v>186.65299999999999</v>
       </c>
       <c r="V110" s="1">
+        <v>193.21350000000001</v>
+      </c>
+      <c r="W110" s="1">
         <v>185.8903</v>
       </c>
-      <c r="W110" s="1">
-        <v>191.78620000000001</v>
-      </c>
-    </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X110" s="1">
+        <v>193.9761</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>534.66</v>
       </c>
@@ -7949,16 +8274,19 @@
         <v>216.9179</v>
       </c>
       <c r="U111" s="1">
-        <v>194.35730000000001</v>
+        <v>187.04740000000001</v>
       </c>
       <c r="V111" s="1">
+        <v>196.2689</v>
+      </c>
+      <c r="W111" s="1">
         <v>185.83250000000001</v>
       </c>
-      <c r="W111" s="1">
-        <v>194.35730000000001</v>
-      </c>
-    </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X111" s="1">
+        <v>197.4838</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>534.55999999999995</v>
       </c>
@@ -8014,16 +8342,19 @@
         <v>224.0369</v>
       </c>
       <c r="U112" s="1">
-        <v>197.97649999999999</v>
+        <v>187.67910000000001</v>
       </c>
       <c r="V112" s="1">
+        <v>200.43270000000001</v>
+      </c>
+      <c r="W112" s="1">
         <v>185.77459999999999</v>
       </c>
-      <c r="W112" s="1">
-        <v>197.97649999999999</v>
-      </c>
-    </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X112" s="1">
+        <v>202.3372</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>534.46</v>
       </c>
@@ -8079,16 +8410,19 @@
         <v>233.24959999999999</v>
       </c>
       <c r="U113" s="1">
-        <v>203.0069</v>
+        <v>188.65649999999999</v>
       </c>
       <c r="V113" s="1">
+        <v>206.01820000000001</v>
+      </c>
+      <c r="W113" s="1">
         <v>185.7166</v>
       </c>
-      <c r="W113" s="1">
-        <v>203.0069</v>
-      </c>
-    </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X113" s="1">
+        <v>208.958</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>534.36</v>
       </c>
@@ -8144,16 +8478,19 @@
         <v>233.66829999999999</v>
       </c>
       <c r="U114" s="1">
-        <v>209.91499999999999</v>
+        <v>190.1694</v>
       </c>
       <c r="V114" s="1">
+        <v>213.5274</v>
+      </c>
+      <c r="W114" s="1">
         <v>185.65860000000001</v>
       </c>
-      <c r="W114" s="1">
-        <v>209.91499999999999</v>
-      </c>
-    </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X114" s="1">
+        <v>218.03829999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>534.26</v>
       </c>
@@ -8209,16 +8546,19 @@
         <v>244.55609999999999</v>
       </c>
       <c r="U115" s="1">
-        <v>219.2912</v>
+        <v>192.4211</v>
       </c>
       <c r="V115" s="1">
+        <v>223.31899999999999</v>
+      </c>
+      <c r="W115" s="1">
         <v>185.60050000000001</v>
       </c>
-      <c r="W115" s="1">
-        <v>219.2912</v>
-      </c>
-    </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X115" s="1">
+        <v>230.1397</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>534.16</v>
       </c>
@@ -8274,16 +8614,19 @@
         <v>273.86930000000001</v>
       </c>
       <c r="U116" s="1">
-        <v>231.8716</v>
+        <v>195.70359999999999</v>
       </c>
       <c r="V116" s="1">
+        <v>235.8837</v>
+      </c>
+      <c r="W116" s="1">
         <v>185.54230000000001</v>
       </c>
-      <c r="W116" s="1">
-        <v>231.8716</v>
-      </c>
-    </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X116" s="1">
+        <v>246.04509999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A117" s="1">
         <v>534.05999999999995</v>
       </c>
@@ -8339,16 +8682,19 @@
         <v>285.59460000000001</v>
       </c>
       <c r="U117" s="1">
-        <v>248.56010000000001</v>
+        <v>200.50559999999999</v>
       </c>
       <c r="V117" s="1">
+        <v>251.9666</v>
+      </c>
+      <c r="W117" s="1">
         <v>185.48410000000001</v>
       </c>
-      <c r="W117" s="1">
-        <v>248.56010000000001</v>
-      </c>
-    </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X117" s="1">
+        <v>266.98809999999997</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A118" s="1">
         <v>533.96</v>
       </c>
@@ -8404,16 +8750,19 @@
         <v>293.96980000000002</v>
       </c>
       <c r="U118" s="1">
-        <v>270.44709999999998</v>
+        <v>207.33330000000001</v>
       </c>
       <c r="V118" s="1">
+        <v>272.00409999999999</v>
+      </c>
+      <c r="W118" s="1">
         <v>185.42590000000001</v>
       </c>
-      <c r="W118" s="1">
-        <v>270.44709999999998</v>
-      </c>
-    </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X118" s="1">
+        <v>293.91149999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A119" s="1">
         <v>533.86</v>
       </c>
@@ -8469,16 +8818,19 @@
         <v>344.63990000000001</v>
       </c>
       <c r="U119" s="1">
-        <v>298.92529999999999</v>
+        <v>216.86019999999999</v>
       </c>
       <c r="V119" s="1">
+        <v>296.51690000000002</v>
+      </c>
+      <c r="W119" s="1">
         <v>185.36770000000001</v>
       </c>
-      <c r="W119" s="1">
-        <v>298.92529999999999</v>
-      </c>
-    </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X119" s="1">
+        <v>328.0093</v>
+      </c>
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A120" s="1">
         <v>533.76</v>
       </c>
@@ -8534,16 +8886,19 @@
         <v>368.928</v>
       </c>
       <c r="U120" s="1">
-        <v>335.51780000000002</v>
+        <v>230.1662</v>
       </c>
       <c r="V120" s="1">
+        <v>326.24979999999999</v>
+      </c>
+      <c r="W120" s="1">
         <v>185.30950000000001</v>
       </c>
-      <c r="W120" s="1">
-        <v>335.51780000000002</v>
-      </c>
-    </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X120" s="1">
+        <v>371.10649999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A121" s="1">
         <v>533.66</v>
       </c>
@@ -8599,16 +8954,19 @@
         <v>420.01679999999999</v>
       </c>
       <c r="U121" s="1">
-        <v>381.8827</v>
+        <v>248.3287</v>
       </c>
       <c r="V121" s="1">
+        <v>361.39319999999998</v>
+      </c>
+      <c r="W121" s="1">
         <v>185.25149999999999</v>
       </c>
-      <c r="W121" s="1">
-        <v>381.8827</v>
-      </c>
-    </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X121" s="1">
+        <v>424.47039999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A122" s="1">
         <v>533.55999999999995</v>
       </c>
@@ -8664,16 +9022,19 @@
         <v>500</v>
       </c>
       <c r="U122" s="1">
-        <v>439.91070000000002</v>
+        <v>272.64729999999997</v>
       </c>
       <c r="V122" s="1">
+        <v>402.02809999999999</v>
+      </c>
+      <c r="W122" s="1">
         <v>185.1935</v>
       </c>
-      <c r="W122" s="1">
-        <v>439.91070000000002</v>
-      </c>
-    </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X122" s="1">
+        <v>489.4819</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A123" s="1">
         <v>533.46</v>
       </c>
@@ -8729,16 +9090,19 @@
         <v>583.33330000000001</v>
       </c>
       <c r="U123" s="1">
-        <v>511.6223</v>
+        <v>305.12110000000001</v>
       </c>
       <c r="V123" s="1">
+        <v>448.23340000000002</v>
+      </c>
+      <c r="W123" s="1">
         <v>185.13579999999999</v>
       </c>
-      <c r="W123" s="1">
-        <v>511.6223</v>
-      </c>
-    </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X123" s="1">
+        <v>568.21870000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A124" s="1">
         <v>533.36</v>
       </c>
@@ -8794,16 +9158,19 @@
         <v>675.04190000000006</v>
       </c>
       <c r="U124" s="1">
-        <v>599.09109999999998</v>
+        <v>347.64179999999999</v>
       </c>
       <c r="V124" s="1">
+        <v>499.30189999999999</v>
+      </c>
+      <c r="W124" s="1">
         <v>185.07839999999999</v>
       </c>
-      <c r="W124" s="1">
-        <v>599.09109999999998</v>
-      </c>
-    </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X124" s="1">
+        <v>661.86530000000005</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A125" s="1">
         <v>533.26</v>
       </c>
@@ -8859,16 +9226,19 @@
         <v>764.65660000000003</v>
       </c>
       <c r="U125" s="1">
-        <v>704.33389999999997</v>
+        <v>402.1927</v>
       </c>
       <c r="V125" s="1">
+        <v>554.15160000000003</v>
+      </c>
+      <c r="W125" s="1">
         <v>185.0213</v>
       </c>
-      <c r="W125" s="1">
-        <v>704.33389999999997</v>
-      </c>
-    </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X125" s="1">
+        <v>771.32299999999998</v>
+      </c>
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A126" s="1">
         <v>533.16</v>
       </c>
@@ -8924,16 +9294,19 @@
         <v>917.50419999999997</v>
       </c>
       <c r="U126" s="1">
-        <v>829.16240000000005</v>
+        <v>471.69749999999999</v>
       </c>
       <c r="V126" s="1">
+        <v>611.33349999999996</v>
+      </c>
+      <c r="W126" s="1">
         <v>184.96469999999999</v>
       </c>
-      <c r="W126" s="1">
-        <v>829.16240000000005</v>
-      </c>
-    </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X126" s="1">
+        <v>898.06629999999996</v>
+      </c>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A127" s="1">
         <v>533.05999999999995</v>
       </c>
@@ -8989,16 +9362,19 @@
         <v>1025.126</v>
       </c>
       <c r="U127" s="1">
-        <v>974.99670000000003</v>
+        <v>558.66700000000003</v>
       </c>
       <c r="V127" s="1">
+        <v>668.68910000000005</v>
+      </c>
+      <c r="W127" s="1">
         <v>184.90870000000001</v>
       </c>
-      <c r="W127" s="1">
-        <v>974.99670000000003</v>
-      </c>
-    </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X127" s="1">
+        <v>1042.4469999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A128" s="1">
         <v>532.96</v>
       </c>
@@ -9054,16 +9430,19 @@
         <v>1179.229</v>
       </c>
       <c r="U128" s="1">
-        <v>1142.6420000000001</v>
+        <v>665.09630000000004</v>
       </c>
       <c r="V128" s="1">
+        <v>723.76059999999995</v>
+      </c>
+      <c r="W128" s="1">
         <v>184.85339999999999</v>
       </c>
-      <c r="W128" s="1">
-        <v>1142.6420000000001</v>
-      </c>
-    </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X128" s="1">
+        <v>1204.0029999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A129" s="1">
         <v>532.86</v>
       </c>
@@ -9119,16 +9498,19 @@
         <v>1365.9970000000001</v>
       </c>
       <c r="U129" s="1">
-        <v>1332.037</v>
+        <v>793.80050000000006</v>
       </c>
       <c r="V129" s="1">
+        <v>773.61260000000004</v>
+      </c>
+      <c r="W129" s="1">
         <v>184.79900000000001</v>
       </c>
-      <c r="W129" s="1">
-        <v>1332.037</v>
-      </c>
-    </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X129" s="1">
+        <v>1382.614</v>
+      </c>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A130" s="1">
         <v>532.76</v>
       </c>
@@ -9184,16 +9566,19 @@
         <v>1597.99</v>
       </c>
       <c r="U130" s="1">
-        <v>1542.296</v>
+        <v>946.51239999999996</v>
       </c>
       <c r="V130" s="1">
+        <v>815.33249999999998</v>
+      </c>
+      <c r="W130" s="1">
         <v>184.7456</v>
       </c>
-      <c r="W130" s="1">
-        <v>1542.296</v>
-      </c>
-    </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X130" s="1">
+        <v>1577.0989999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A131" s="1">
         <v>532.66</v>
       </c>
@@ -9249,16 +9634,19 @@
         <v>1762.144</v>
       </c>
       <c r="U131" s="1">
-        <v>1770.4870000000001</v>
+        <v>1123.1959999999999</v>
       </c>
       <c r="V131" s="1">
+        <v>846.56140000000005</v>
+      </c>
+      <c r="W131" s="1">
         <v>184.6934</v>
       </c>
-      <c r="W131" s="1">
-        <v>1770.4870000000001</v>
-      </c>
-    </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X131" s="1">
+        <v>1785.0640000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A132" s="1">
         <v>532.55999999999995</v>
       </c>
@@ -9314,16 +9702,19 @@
         <v>1985.3430000000001</v>
       </c>
       <c r="U132" s="1">
-        <v>2012.2850000000001</v>
+        <v>1323.826</v>
       </c>
       <c r="V132" s="1">
+        <v>864.89030000000002</v>
+      </c>
+      <c r="W132" s="1">
         <v>184.64259999999999</v>
       </c>
-      <c r="W132" s="1">
-        <v>2012.2850000000001</v>
-      </c>
-    </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X132" s="1">
+        <v>2004.0740000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A133" s="1">
         <v>532.46</v>
       </c>
@@ -9379,16 +9770,19 @@
         <v>2198.0740000000001</v>
       </c>
       <c r="U133" s="1">
-        <v>2261.7809999999999</v>
+        <v>1546.26</v>
       </c>
       <c r="V133" s="1">
+        <v>868.94539999999995</v>
+      </c>
+      <c r="W133" s="1">
         <v>184.5934</v>
       </c>
-      <c r="W133" s="1">
-        <v>2261.7809999999999</v>
-      </c>
-    </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X133" s="1">
+        <v>2230.6120000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A134" s="1">
         <v>532.36</v>
       </c>
@@ -9444,16 +9838,19 @@
         <v>2461.0549999999998</v>
       </c>
       <c r="U134" s="1">
-        <v>2511.4450000000002</v>
+        <v>1785.384</v>
       </c>
       <c r="V134" s="1">
+        <v>858.87699999999995</v>
+      </c>
+      <c r="W134" s="1">
         <v>184.54599999999999</v>
       </c>
-      <c r="W134" s="1">
-        <v>2511.4450000000002</v>
-      </c>
-    </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X134" s="1">
+        <v>2459.7150000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A135" s="1">
         <v>532.26</v>
       </c>
@@ -9509,16 +9906,19 @@
         <v>2708.9609999999998</v>
       </c>
       <c r="U135" s="1">
-        <v>2752.3580000000002</v>
+        <v>2034.903</v>
       </c>
       <c r="V135" s="1">
+        <v>835.0702</v>
+      </c>
+      <c r="W135" s="1">
         <v>184.50059999999999</v>
       </c>
-      <c r="W135" s="1">
-        <v>2752.3580000000002</v>
-      </c>
-    </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X135" s="1">
+        <v>2685.473</v>
+      </c>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A136" s="1">
         <v>532.16</v>
       </c>
@@ -9574,16 +9974,19 @@
         <v>2930.067</v>
       </c>
       <c r="U136" s="1">
-        <v>2974.654</v>
+        <v>2285.7040000000002</v>
       </c>
       <c r="V136" s="1">
+        <v>799.04259999999999</v>
+      </c>
+      <c r="W136" s="1">
         <v>184.45750000000001</v>
       </c>
-      <c r="W136" s="1">
-        <v>2974.654</v>
-      </c>
-    </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X136" s="1">
+        <v>2900.29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A137" s="1">
         <v>532.05999999999995</v>
       </c>
@@ -9639,16 +10042,19 @@
         <v>3162.06</v>
       </c>
       <c r="U137" s="1">
-        <v>3168.17</v>
+        <v>2526.9189999999999</v>
       </c>
       <c r="V137" s="1">
+        <v>753.55539999999996</v>
+      </c>
+      <c r="W137" s="1">
         <v>184.4169</v>
       </c>
-      <c r="W137" s="1">
-        <v>3168.17</v>
-      </c>
-    </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X137" s="1">
+        <v>3096.0569999999998</v>
+      </c>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A138" s="1">
         <v>531.96</v>
       </c>
@@ -9704,16 +10110,19 @@
         <v>3264.2379999999998</v>
       </c>
       <c r="U138" s="1">
-        <v>3323.24</v>
+        <v>2746.4050000000002</v>
       </c>
       <c r="V138" s="1">
+        <v>701.16849999999999</v>
+      </c>
+      <c r="W138" s="1">
         <v>184.37889999999999</v>
       </c>
-      <c r="W138" s="1">
-        <v>3323.24</v>
-      </c>
-    </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X138" s="1">
+        <v>3263.1950000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A139" s="1">
         <v>531.86</v>
       </c>
@@ -9769,16 +10178,19 @@
         <v>3412.06</v>
       </c>
       <c r="U139" s="1">
-        <v>3431.5749999999998</v>
+        <v>2930.3409999999999</v>
       </c>
       <c r="V139" s="1">
+        <v>644.71950000000004</v>
+      </c>
+      <c r="W139" s="1">
         <v>184.34379999999999</v>
       </c>
-      <c r="W139" s="1">
-        <v>3431.5749999999998</v>
-      </c>
-    </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X139" s="1">
+        <v>3390.7170000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A140" s="1">
         <v>531.76</v>
       </c>
@@ -9834,16 +10246,19 @@
         <v>3462.3119999999999</v>
       </c>
       <c r="U140" s="1">
-        <v>3487.0790000000002</v>
+        <v>3068.8180000000002</v>
       </c>
       <c r="V140" s="1">
+        <v>587.06510000000003</v>
+      </c>
+      <c r="W140" s="1">
         <v>184.3115</v>
       </c>
-      <c r="W140" s="1">
-        <v>3487.0790000000002</v>
-      </c>
-    </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X140" s="1">
+        <v>3471.5720000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A141" s="1">
         <v>531.66</v>
       </c>
@@ -9899,16 +10314,19 @@
         <v>3466.08</v>
       </c>
       <c r="U141" s="1">
-        <v>3485.3470000000002</v>
+        <v>3152.404</v>
       </c>
       <c r="V141" s="1">
+        <v>530.49130000000002</v>
+      </c>
+      <c r="W141" s="1">
         <v>184.28219999999999</v>
       </c>
-      <c r="W141" s="1">
-        <v>3485.3470000000002</v>
-      </c>
-    </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X141" s="1">
+        <v>3498.6129999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A142" s="1">
         <v>531.55999999999995</v>
       </c>
@@ -9964,16 +10382,19 @@
         <v>3401.1729999999998</v>
       </c>
       <c r="U142" s="1">
-        <v>3427.6010000000001</v>
+        <v>3172.6869999999999</v>
       </c>
       <c r="V142" s="1">
+        <v>476.99290000000002</v>
+      </c>
+      <c r="W142" s="1">
         <v>184.25579999999999</v>
       </c>
-      <c r="W142" s="1">
-        <v>3427.6010000000001</v>
-      </c>
-    </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X142" s="1">
+        <v>3465.424</v>
+      </c>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A143" s="1">
         <v>531.46</v>
       </c>
@@ -10029,16 +10450,19 @@
         <v>3324.5390000000002</v>
       </c>
       <c r="U143" s="1">
-        <v>3317.2269999999999</v>
+        <v>3131.2719999999999</v>
       </c>
       <c r="V143" s="1">
+        <v>427.7602</v>
+      </c>
+      <c r="W143" s="1">
         <v>184.23240000000001</v>
       </c>
-      <c r="W143" s="1">
-        <v>3317.2269999999999</v>
-      </c>
-    </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X143" s="1">
+        <v>3374.799</v>
+      </c>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A144" s="1">
         <v>531.36</v>
       </c>
@@ -10094,16 +10518,19 @@
         <v>3228.2240000000002</v>
       </c>
       <c r="U144" s="1">
-        <v>3160.4119999999998</v>
+        <v>3030.721</v>
       </c>
       <c r="V144" s="1">
+        <v>383.63150000000002</v>
+      </c>
+      <c r="W144" s="1">
         <v>184.21180000000001</v>
       </c>
-      <c r="W144" s="1">
-        <v>3160.4119999999998</v>
-      </c>
-    </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X144" s="1">
+        <v>3230.1410000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A145" s="1">
         <v>531.26</v>
       </c>
@@ -10159,16 +10586,19 @@
         <v>3059.4639999999999</v>
       </c>
       <c r="U145" s="1">
-        <v>2965.509</v>
+        <v>2875.3710000000001</v>
       </c>
       <c r="V145" s="1">
+        <v>345.23379999999997</v>
+      </c>
+      <c r="W145" s="1">
         <v>184.19390000000001</v>
       </c>
-      <c r="W145" s="1">
-        <v>2965.509</v>
-      </c>
-    </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X145" s="1">
+        <v>3036.4110000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A146" s="1">
         <v>531.16</v>
       </c>
@@ -10224,16 +10654,19 @@
         <v>2822.027</v>
       </c>
       <c r="U146" s="1">
-        <v>2742.2150000000001</v>
+        <v>2678.337</v>
       </c>
       <c r="V146" s="1">
+        <v>312.29860000000002</v>
+      </c>
+      <c r="W146" s="1">
         <v>184.17869999999999</v>
       </c>
-      <c r="W146" s="1">
-        <v>2742.2150000000001</v>
-      </c>
-    </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X146" s="1">
+        <v>2806.4569999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A147" s="1">
         <v>531.05999999999995</v>
       </c>
@@ -10289,16 +10722,19 @@
         <v>2558.2080000000001</v>
       </c>
       <c r="U147" s="1">
-        <v>2500.6970000000001</v>
+        <v>2451.0859999999998</v>
       </c>
       <c r="V147" s="1">
+        <v>284.60329999999999</v>
+      </c>
+      <c r="W147" s="1">
         <v>184.16579999999999</v>
       </c>
-      <c r="W147" s="1">
-        <v>2500.6970000000001</v>
-      </c>
-    </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X147" s="1">
+        <v>2551.5230000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A148" s="1">
         <v>530.96</v>
       </c>
@@ -10354,16 +10790,19 @@
         <v>2316.5830000000001</v>
       </c>
       <c r="U148" s="1">
-        <v>2250.7950000000001</v>
+        <v>2205.1669999999999</v>
       </c>
       <c r="V148" s="1">
+        <v>261.9726</v>
+      </c>
+      <c r="W148" s="1">
         <v>184.1551</v>
       </c>
-      <c r="W148" s="1">
-        <v>2250.7950000000001</v>
-      </c>
-    </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X148" s="1">
+        <v>2282.9839999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A149" s="1">
         <v>530.86</v>
       </c>
@@ -10419,16 +10858,19 @@
         <v>2052.7640000000001</v>
       </c>
       <c r="U149" s="1">
-        <v>2001.383</v>
+        <v>1953.597</v>
       </c>
       <c r="V149" s="1">
+        <v>243.58959999999999</v>
+      </c>
+      <c r="W149" s="1">
         <v>184.1463</v>
       </c>
-      <c r="W149" s="1">
-        <v>2001.383</v>
-      </c>
-    </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X149" s="1">
+        <v>2013.04</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A150" s="1">
         <v>530.76</v>
       </c>
@@ -10484,16 +10926,19 @@
         <v>1773.451</v>
       </c>
       <c r="U150" s="1">
-        <v>1759.9380000000001</v>
+        <v>1706.249</v>
       </c>
       <c r="V150" s="1">
+        <v>228.898</v>
+      </c>
+      <c r="W150" s="1">
         <v>184.13919999999999</v>
       </c>
-      <c r="W150" s="1">
-        <v>1759.9380000000001</v>
-      </c>
-    </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X150" s="1">
+        <v>1751.0070000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A151" s="1">
         <v>530.66</v>
       </c>
@@ -10549,16 +10994,19 @@
         <v>1530.1510000000001</v>
       </c>
       <c r="U151" s="1">
-        <v>1532.366</v>
+        <v>1472.068</v>
       </c>
       <c r="V151" s="1">
+        <v>217.49889999999999</v>
+      </c>
+      <c r="W151" s="1">
         <v>184.1336</v>
       </c>
-      <c r="W151" s="1">
-        <v>1532.366</v>
-      </c>
-    </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X151" s="1">
+        <v>1505.433</v>
+      </c>
+    </row>
+    <row r="152" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A152" s="1">
         <v>530.55999999999995</v>
       </c>
@@ -10614,16 +11062,19 @@
         <v>1276.3820000000001</v>
       </c>
       <c r="U152" s="1">
-        <v>1323.1590000000001</v>
+        <v>1256.423</v>
       </c>
       <c r="V152" s="1">
+        <v>208.66059999999999</v>
+      </c>
+      <c r="W152" s="1">
         <v>184.1292</v>
       </c>
-      <c r="W152" s="1">
-        <v>1323.1590000000001</v>
-      </c>
-    </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X152" s="1">
+        <v>1280.954</v>
+      </c>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A153" s="1">
         <v>530.46</v>
       </c>
@@ -10679,16 +11130,19 @@
         <v>1068.258</v>
       </c>
       <c r="U153" s="1">
-        <v>1134.5730000000001</v>
+        <v>1062.7570000000001</v>
       </c>
       <c r="V153" s="1">
+        <v>201.9058</v>
+      </c>
+      <c r="W153" s="1">
         <v>184.12569999999999</v>
       </c>
-      <c r="W153" s="1">
-        <v>1134.5730000000001</v>
-      </c>
-    </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X153" s="1">
+        <v>1080.537</v>
+      </c>
+    </row>
+    <row r="154" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A154" s="1">
         <v>530.36</v>
       </c>
@@ -10744,16 +11198,19 @@
         <v>904.10389999999995</v>
       </c>
       <c r="U154" s="1">
-        <v>967.75289999999995</v>
+        <v>894.00350000000003</v>
       </c>
       <c r="V154" s="1">
+        <v>196.89179999999999</v>
+      </c>
+      <c r="W154" s="1">
         <v>184.12309999999999</v>
       </c>
-      <c r="W154" s="1">
-        <v>967.75289999999995</v>
-      </c>
-    </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X154" s="1">
+        <v>906.7722</v>
+      </c>
+    </row>
+    <row r="155" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A155" s="1">
         <v>530.26</v>
       </c>
@@ -10809,16 +11266,19 @@
         <v>715.24289999999996</v>
       </c>
       <c r="U155" s="1">
-        <v>822.72320000000002</v>
+        <v>749.36829999999998</v>
       </c>
       <c r="V155" s="1">
+        <v>193.1694</v>
+      </c>
+      <c r="W155" s="1">
         <v>184.12110000000001</v>
       </c>
-      <c r="W155" s="1">
-        <v>822.72320000000002</v>
-      </c>
-    </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X155" s="1">
+        <v>758.41660000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A156" s="1">
         <v>530.16</v>
       </c>
@@ -10874,16 +11334,19 @@
         <v>617.67169999999999</v>
       </c>
       <c r="U156" s="1">
-        <v>698.65250000000003</v>
+        <v>627.57759999999996</v>
       </c>
       <c r="V156" s="1">
+        <v>190.43899999999999</v>
+      </c>
+      <c r="W156" s="1">
         <v>184.11959999999999</v>
       </c>
-      <c r="W156" s="1">
-        <v>698.65250000000003</v>
-      </c>
-    </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X156" s="1">
+        <v>633.89700000000005</v>
+      </c>
+    </row>
+    <row r="157" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A157" s="1">
         <v>530.05999999999995</v>
       </c>
@@ -10939,16 +11402,19 @@
         <v>507.95639999999997</v>
       </c>
       <c r="U157" s="1">
-        <v>594.10310000000004</v>
+        <v>527.73429999999996</v>
       </c>
       <c r="V157" s="1">
+        <v>188.49340000000001</v>
+      </c>
+      <c r="W157" s="1">
         <v>184.11850000000001</v>
       </c>
-      <c r="W157" s="1">
-        <v>594.10310000000004</v>
-      </c>
-    </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X157" s="1">
+        <v>532.10919999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A158" s="1">
         <v>529.96</v>
       </c>
@@ -11004,16 +11470,19 @@
         <v>404.10390000000001</v>
       </c>
       <c r="U158" s="1">
-        <v>507.25229999999999</v>
+        <v>446.84339999999997</v>
       </c>
       <c r="V158" s="1">
+        <v>187.10769999999999</v>
+      </c>
+      <c r="W158" s="1">
         <v>184.11770000000001</v>
       </c>
-      <c r="W158" s="1">
-        <v>507.25229999999999</v>
-      </c>
-    </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X158" s="1">
+        <v>449.83350000000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A159" s="1">
         <v>529.86</v>
       </c>
@@ -11069,16 +11538,19 @@
         <v>356.36520000000002</v>
       </c>
       <c r="U159" s="1">
-        <v>436.0788</v>
+        <v>382.1463</v>
       </c>
       <c r="V159" s="1">
+        <v>186.13030000000001</v>
+      </c>
+      <c r="W159" s="1">
         <v>184.11709999999999</v>
       </c>
-      <c r="W159" s="1">
-        <v>436.0788</v>
-      </c>
-    </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X159" s="1">
+        <v>384.15949999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A160" s="1">
         <v>529.76</v>
       </c>
@@ -11134,16 +11606,19 @@
         <v>315.74540000000002</v>
       </c>
       <c r="U160" s="1">
-        <v>378.50909999999999</v>
+        <v>331.67840000000001</v>
       </c>
       <c r="V160" s="1">
+        <v>185.46039999999999</v>
+      </c>
+      <c r="W160" s="1">
         <v>184.11660000000001</v>
       </c>
-      <c r="W160" s="1">
-        <v>378.50909999999999</v>
-      </c>
-    </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X160" s="1">
+        <v>333.02210000000002</v>
+      </c>
+    </row>
+    <row r="161" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A161" s="1">
         <v>529.66</v>
       </c>
@@ -11199,16 +11674,19 @@
         <v>272.61309999999997</v>
       </c>
       <c r="U161" s="1">
-        <v>332.52609999999999</v>
+        <v>292.72149999999999</v>
       </c>
       <c r="V161" s="1">
+        <v>185.00229999999999</v>
+      </c>
+      <c r="W161" s="1">
         <v>184.1163</v>
       </c>
-      <c r="W161" s="1">
-        <v>332.52609999999999</v>
-      </c>
-    </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X161" s="1">
+        <v>293.60759999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A162" s="1">
         <v>529.55999999999995</v>
       </c>
@@ -11264,16 +11742,19 @@
         <v>243.71860000000001</v>
       </c>
       <c r="U162" s="1">
-        <v>296.30439999999999</v>
+        <v>262.92410000000001</v>
       </c>
       <c r="V162" s="1">
+        <v>184.69130000000001</v>
+      </c>
+      <c r="W162" s="1">
         <v>184.11600000000001</v>
       </c>
-      <c r="W162" s="1">
-        <v>296.30439999999999</v>
-      </c>
-    </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X162" s="1">
+        <v>263.49930000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A163" s="1">
         <v>529.46</v>
       </c>
@@ -11329,16 +11810,19 @@
         <v>237.85589999999999</v>
       </c>
       <c r="U163" s="1">
-        <v>268.14499999999998</v>
+        <v>240.67070000000001</v>
       </c>
       <c r="V163" s="1">
+        <v>184.48589999999999</v>
+      </c>
+      <c r="W163" s="1">
         <v>184.11580000000001</v>
       </c>
-      <c r="W163" s="1">
-        <v>268.14499999999998</v>
-      </c>
-    </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X163" s="1">
+        <v>241.04089999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A164" s="1">
         <v>529.36</v>
       </c>
@@ -11394,16 +11878,19 @@
         <v>221.94300000000001</v>
       </c>
       <c r="U164" s="1">
-        <v>246.4239</v>
+        <v>224.23859999999999</v>
       </c>
       <c r="V164" s="1">
+        <v>184.3511</v>
+      </c>
+      <c r="W164" s="1">
         <v>184.1157</v>
       </c>
-      <c r="W164" s="1">
-        <v>246.4239</v>
-      </c>
-    </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X164" s="1">
+        <v>224.47399999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A165" s="1">
         <v>529.26</v>
       </c>
@@ -11459,16 +11946,19 @@
         <v>202.68010000000001</v>
       </c>
       <c r="U165" s="1">
-        <v>229.85669999999999</v>
+        <v>212.1748</v>
       </c>
       <c r="V165" s="1">
+        <v>184.26300000000001</v>
+      </c>
+      <c r="W165" s="1">
         <v>184.1155</v>
       </c>
-      <c r="W165" s="1">
-        <v>229.85669999999999</v>
-      </c>
-    </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X165" s="1">
+        <v>212.32220000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A166" s="1">
         <v>529.16</v>
       </c>
@@ -11524,16 +12014,19 @@
         <v>196.39869999999999</v>
       </c>
       <c r="U166" s="1">
-        <v>217.36009999999999</v>
+        <v>203.52</v>
       </c>
       <c r="V166" s="1">
+        <v>184.20679999999999</v>
+      </c>
+      <c r="W166" s="1">
         <v>184.11539999999999</v>
       </c>
-      <c r="W166" s="1">
-        <v>217.36009999999999</v>
-      </c>
-    </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X166" s="1">
+        <v>203.6114</v>
+      </c>
+    </row>
+    <row r="167" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A167" s="1">
         <v>529.05999999999995</v>
       </c>
@@ -11589,16 +12082,19 @@
         <v>214.40539999999999</v>
       </c>
       <c r="U167" s="1">
-        <v>208.0368</v>
+        <v>197.3946</v>
       </c>
       <c r="V167" s="1">
+        <v>184.17140000000001</v>
+      </c>
+      <c r="W167" s="1">
         <v>184.11529999999999</v>
       </c>
-      <c r="W167" s="1">
-        <v>208.0368</v>
-      </c>
-    </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X167" s="1">
+        <v>197.45070000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A168" s="1">
         <v>528.96</v>
       </c>
@@ -11654,16 +12150,19 @@
         <v>197.2362</v>
       </c>
       <c r="U168" s="1">
-        <v>201.15649999999999</v>
+        <v>193.06979999999999</v>
       </c>
       <c r="V168" s="1">
+        <v>184.1491</v>
+      </c>
+      <c r="W168" s="1">
         <v>184.11529999999999</v>
       </c>
-      <c r="W168" s="1">
-        <v>201.15649999999999</v>
-      </c>
-    </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X168" s="1">
+        <v>193.1037</v>
+      </c>
+    </row>
+    <row r="169" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A169" s="1">
         <v>528.86</v>
       </c>
@@ -11719,16 +12218,19 @@
         <v>188.86099999999999</v>
       </c>
       <c r="U169" s="1">
-        <v>196.1336</v>
+        <v>190.08349999999999</v>
       </c>
       <c r="V169" s="1">
+        <v>184.1354</v>
+      </c>
+      <c r="W169" s="1">
         <v>184.11519999999999</v>
       </c>
-      <c r="W169" s="1">
-        <v>196.1336</v>
-      </c>
-    </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X169" s="1">
+        <v>190.10380000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A170" s="1">
         <v>528.76</v>
       </c>
@@ -11784,16 +12286,19 @@
         <v>195.14240000000001</v>
       </c>
       <c r="U170" s="1">
-        <v>192.50620000000001</v>
+        <v>188.05619999999999</v>
       </c>
       <c r="V170" s="1">
+        <v>184.12710000000001</v>
+      </c>
+      <c r="W170" s="1">
         <v>184.11519999999999</v>
       </c>
-      <c r="W170" s="1">
-        <v>192.50620000000001</v>
-      </c>
-    </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X170" s="1">
+        <v>188.06819999999999</v>
+      </c>
+    </row>
+    <row r="171" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A171" s="1">
         <v>528.66</v>
       </c>
@@ -11849,16 +12354,19 @@
         <v>190.1173</v>
       </c>
       <c r="U171" s="1">
-        <v>189.9144</v>
+        <v>186.6781</v>
       </c>
       <c r="V171" s="1">
+        <v>184.12209999999999</v>
+      </c>
+      <c r="W171" s="1">
         <v>184.11510000000001</v>
       </c>
-      <c r="W171" s="1">
-        <v>189.9144</v>
-      </c>
-    </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X171" s="1">
+        <v>186.68510000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A172" s="1">
         <v>528.55999999999995</v>
       </c>
@@ -11914,16 +12422,19 @@
         <v>189.6985</v>
       </c>
       <c r="U172" s="1">
-        <v>188.08250000000001</v>
+        <v>185.7612</v>
       </c>
       <c r="V172" s="1">
+        <v>184.1191</v>
+      </c>
+      <c r="W172" s="1">
         <v>184.11510000000001</v>
       </c>
-      <c r="W172" s="1">
-        <v>188.08250000000001</v>
-      </c>
-    </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X172" s="1">
+        <v>185.76519999999999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A173" s="1">
         <v>528.46</v>
       </c>
@@ -11979,16 +12490,19 @@
         <v>193.04859999999999</v>
       </c>
       <c r="U173" s="1">
-        <v>186.80600000000001</v>
+        <v>185.16399999999999</v>
       </c>
       <c r="V173" s="1">
+        <v>184.1173</v>
+      </c>
+      <c r="W173" s="1">
         <v>184.11510000000001</v>
       </c>
-      <c r="W173" s="1">
-        <v>186.80600000000001</v>
-      </c>
-    </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X173" s="1">
+        <v>185.16630000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A174" s="1">
         <v>528.36</v>
       </c>
@@ -12044,16 +12558,19 @@
         <v>200.58629999999999</v>
       </c>
       <c r="U174" s="1">
-        <v>185.9246</v>
+        <v>184.773</v>
       </c>
       <c r="V174" s="1">
+        <v>184.1163</v>
+      </c>
+      <c r="W174" s="1">
         <v>184.11500000000001</v>
       </c>
-      <c r="W174" s="1">
-        <v>185.9246</v>
-      </c>
-    </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X174" s="1">
+        <v>184.77420000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A175" s="1">
         <v>528.26</v>
       </c>
@@ -12109,16 +12626,19 @@
         <v>184.25460000000001</v>
       </c>
       <c r="U175" s="1">
-        <v>185.31979999999999</v>
+        <v>184.52209999999999</v>
       </c>
       <c r="V175" s="1">
+        <v>184.1157</v>
+      </c>
+      <c r="W175" s="1">
         <v>184.11500000000001</v>
       </c>
-      <c r="W175" s="1">
-        <v>185.31979999999999</v>
-      </c>
-    </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X175" s="1">
+        <v>184.52279999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A176" s="1">
         <v>528.16</v>
       </c>
@@ -12174,16 +12694,19 @@
         <v>191.79230000000001</v>
       </c>
       <c r="U176" s="1">
-        <v>184.9092</v>
+        <v>184.36529999999999</v>
       </c>
       <c r="V176" s="1">
+        <v>184.11539999999999</v>
+      </c>
+      <c r="W176" s="1">
         <v>184.11500000000001</v>
       </c>
-      <c r="W176" s="1">
-        <v>184.9092</v>
-      </c>
-    </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X176" s="1">
+        <v>184.3657</v>
+      </c>
+    </row>
+    <row r="177" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A177" s="1">
         <v>528.05999999999995</v>
       </c>
@@ -12239,16 +12762,19 @@
         <v>180.90450000000001</v>
       </c>
       <c r="U177" s="1">
-        <v>184.63319999999999</v>
+        <v>184.2664</v>
       </c>
       <c r="V177" s="1">
+        <v>184.11519999999999</v>
+      </c>
+      <c r="W177" s="1">
         <v>184.11500000000001</v>
       </c>
-      <c r="W177" s="1">
-        <v>184.63319999999999</v>
-      </c>
-    </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X177" s="1">
+        <v>184.26660000000001</v>
+      </c>
+    </row>
+    <row r="178" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A178" s="1">
         <v>527.96</v>
       </c>
@@ -12304,16 +12830,19 @@
         <v>179.6482</v>
       </c>
       <c r="U178" s="1">
-        <v>179.983</v>
+        <v>179.73840000000001</v>
       </c>
       <c r="V178" s="1">
+        <v>179.64840000000001</v>
+      </c>
+      <c r="W178" s="1">
         <v>179.6482</v>
       </c>
-      <c r="W178" s="1">
-        <v>179.983</v>
-      </c>
-    </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="X178" s="1">
+        <v>179.73859999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A179" s="1">
         <v>527.86</v>
       </c>
@@ -12369,16 +12898,19 @@
         <v>181.32329999999999</v>
       </c>
       <c r="U179" s="1">
-        <v>181.53729999999999</v>
+        <v>181.3768</v>
       </c>
       <c r="V179" s="1">
         <v>181.32329999999999</v>
       </c>
       <c r="W179" s="1">
-        <v>181.53729999999999</v>
-      </c>
-    </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.45">
+        <v>181.32329999999999</v>
+      </c>
+      <c r="X179" s="1">
+        <v>181.37690000000001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A180" s="1">
         <v>527.76</v>
       </c>
@@ -12434,16 +12966,19 @@
         <v>175.8794</v>
       </c>
       <c r="U180" s="1">
-        <v>176.01480000000001</v>
+        <v>175.91059999999999</v>
       </c>
       <c r="V180" s="1">
         <v>175.8794</v>
       </c>
       <c r="W180" s="1">
-        <v>176.01480000000001</v>
-      </c>
-    </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.45">
+        <v>175.8794</v>
+      </c>
+      <c r="X180" s="1">
+        <v>175.91069999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A181" s="1">
         <v>527.66</v>
       </c>
@@ -12499,16 +13034,19 @@
         <v>169.59800000000001</v>
       </c>
       <c r="U181" s="1">
-        <v>169.68279999999999</v>
+        <v>169.61590000000001</v>
       </c>
       <c r="V181" s="1">
         <v>169.59800000000001</v>
       </c>
       <c r="W181" s="1">
-        <v>169.68279999999999</v>
-      </c>
-    </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.45">
+        <v>169.59800000000001</v>
+      </c>
+      <c r="X181" s="1">
+        <v>169.61590000000001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A182" s="1">
         <v>527.55999999999995</v>
       </c>
@@ -12564,16 +13102,19 @@
         <v>176.71690000000001</v>
       </c>
       <c r="U182" s="1">
-        <v>176.76949999999999</v>
+        <v>176.72720000000001</v>
       </c>
       <c r="V182" s="1">
         <v>176.71690000000001</v>
       </c>
       <c r="W182" s="1">
-        <v>176.76949999999999</v>
-      </c>
-    </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.45">
+        <v>176.71690000000001</v>
+      </c>
+      <c r="X182" s="1">
+        <v>176.72720000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A183" s="1">
         <v>527.46</v>
       </c>
@@ -12629,16 +13170,19 @@
         <v>182.5796</v>
       </c>
       <c r="U183" s="1">
-        <v>182.61179999999999</v>
+        <v>182.58529999999999</v>
       </c>
       <c r="V183" s="1">
         <v>182.5796</v>
       </c>
       <c r="W183" s="1">
-        <v>182.61179999999999</v>
-      </c>
-    </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.45">
+        <v>182.5796</v>
+      </c>
+      <c r="X183" s="1">
+        <v>182.58529999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A184" s="1">
         <v>527.36</v>
       </c>
@@ -12694,16 +13238,19 @@
         <v>192.21109999999999</v>
       </c>
       <c r="U184" s="1">
-        <v>192.23070000000001</v>
+        <v>192.21420000000001</v>
       </c>
       <c r="V184" s="1">
         <v>192.21109999999999</v>
       </c>
       <c r="W184" s="1">
-        <v>192.23070000000001</v>
-      </c>
-    </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.45">
+        <v>192.21109999999999</v>
+      </c>
+      <c r="X184" s="1">
+        <v>192.21420000000001</v>
+      </c>
+    </row>
+    <row r="185" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A185" s="1">
         <v>527.26</v>
       </c>
@@ -12759,16 +13306,19 @@
         <v>181.74199999999999</v>
       </c>
       <c r="U185" s="1">
-        <v>181.75389999999999</v>
+        <v>181.74379999999999</v>
       </c>
       <c r="V185" s="1">
         <v>181.74199999999999</v>
       </c>
       <c r="W185" s="1">
-        <v>181.75389999999999</v>
-      </c>
-    </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.45">
+        <v>181.74199999999999</v>
+      </c>
+      <c r="X185" s="1">
+        <v>181.74379999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A186" s="1">
         <v>527.16</v>
       </c>
@@ -12824,16 +13374,19 @@
         <v>175.4606</v>
       </c>
       <c r="U186" s="1">
-        <v>175.46770000000001</v>
+        <v>175.4616</v>
       </c>
       <c r="V186" s="1">
         <v>175.4606</v>
       </c>
       <c r="W186" s="1">
-        <v>175.46770000000001</v>
-      </c>
-    </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.45">
+        <v>175.4606</v>
+      </c>
+      <c r="X186" s="1">
+        <v>175.4616</v>
+      </c>
+    </row>
+    <row r="187" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A187" s="1">
         <v>527.05999999999995</v>
       </c>
@@ -12889,16 +13442,19 @@
         <v>174.20439999999999</v>
       </c>
       <c r="U187" s="1">
-        <v>174.20849999999999</v>
+        <v>174.20490000000001</v>
       </c>
       <c r="V187" s="1">
         <v>174.20439999999999</v>
       </c>
       <c r="W187" s="1">
-        <v>174.20849999999999</v>
-      </c>
-    </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.45">
+        <v>174.20439999999999</v>
+      </c>
+      <c r="X187" s="1">
+        <v>174.20490000000001</v>
+      </c>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A188" s="1">
         <v>526.96</v>
       </c>
@@ -12954,16 +13510,19 @@
         <v>168.76050000000001</v>
       </c>
       <c r="U188" s="1">
-        <v>168.7629</v>
+        <v>168.76070000000001</v>
       </c>
       <c r="V188" s="1">
         <v>168.76050000000001</v>
       </c>
       <c r="W188" s="1">
-        <v>168.7629</v>
-      </c>
-    </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.45">
+        <v>168.76050000000001</v>
+      </c>
+      <c r="X188" s="1">
+        <v>168.76070000000001</v>
+      </c>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A189" s="1">
         <v>526.86</v>
       </c>
@@ -13019,16 +13578,19 @@
         <v>178.392</v>
       </c>
       <c r="U189" s="1">
-        <v>178.39340000000001</v>
+        <v>178.3921</v>
       </c>
       <c r="V189" s="1">
         <v>178.392</v>
       </c>
       <c r="W189" s="1">
-        <v>178.39340000000001</v>
-      </c>
-    </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.45">
+        <v>178.392</v>
+      </c>
+      <c r="X189" s="1">
+        <v>178.3921</v>
+      </c>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A190" s="1">
         <v>526.76</v>
       </c>
@@ -13084,16 +13646,19 @@
         <v>179.6482</v>
       </c>
       <c r="U190" s="1">
-        <v>179.6491</v>
+        <v>179.64830000000001</v>
       </c>
       <c r="V190" s="1">
         <v>179.6482</v>
       </c>
       <c r="W190" s="1">
-        <v>179.6491</v>
-      </c>
-    </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.45">
+        <v>179.6482</v>
+      </c>
+      <c r="X190" s="1">
+        <v>179.64830000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A191" s="1">
         <v>526.66</v>
       </c>
@@ -13149,16 +13714,19 @@
         <v>179.6482</v>
       </c>
       <c r="U191" s="1">
-        <v>179.64869999999999</v>
+        <v>179.64830000000001</v>
       </c>
       <c r="V191" s="1">
         <v>179.6482</v>
       </c>
       <c r="W191" s="1">
-        <v>179.64869999999999</v>
-      </c>
-    </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.45">
+        <v>179.6482</v>
+      </c>
+      <c r="X191" s="1">
+        <v>179.64830000000001</v>
+      </c>
+    </row>
+    <row r="192" spans="1:24" x14ac:dyDescent="0.45">
       <c r="I192" s="1">
         <v>283.56</v>
       </c>
@@ -13193,16 +13761,19 @@
         <v>174.62309999999999</v>
       </c>
       <c r="U192" s="1">
-        <v>174.6234</v>
+        <v>174.62309999999999</v>
       </c>
       <c r="V192" s="1">
         <v>174.62309999999999</v>
       </c>
       <c r="W192" s="1">
-        <v>174.6234</v>
-      </c>
-    </row>
-    <row r="193" spans="9:23" x14ac:dyDescent="0.45">
+        <v>174.62309999999999</v>
+      </c>
+      <c r="X192" s="1">
+        <v>174.62309999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I193" s="1">
         <v>283.45999999999998</v>
       </c>
@@ -13237,16 +13808,19 @@
         <v>172.52930000000001</v>
       </c>
       <c r="U193" s="1">
-        <v>172.52950000000001</v>
+        <v>172.52930000000001</v>
       </c>
       <c r="V193" s="1">
         <v>172.52930000000001</v>
       </c>
       <c r="W193" s="1">
-        <v>172.52950000000001</v>
-      </c>
-    </row>
-    <row r="194" spans="9:23" x14ac:dyDescent="0.45">
+        <v>172.52930000000001</v>
+      </c>
+      <c r="X193" s="1">
+        <v>172.52930000000001</v>
+      </c>
+    </row>
+    <row r="194" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I194" s="1">
         <v>283.36</v>
       </c>
@@ -13281,16 +13855,19 @@
         <v>173.36680000000001</v>
       </c>
       <c r="U194" s="1">
-        <v>173.36689999999999</v>
+        <v>173.36680000000001</v>
       </c>
       <c r="V194" s="1">
         <v>173.36680000000001</v>
       </c>
       <c r="W194" s="1">
-        <v>173.36689999999999</v>
-      </c>
-    </row>
-    <row r="195" spans="9:23" x14ac:dyDescent="0.45">
+        <v>173.36680000000001</v>
+      </c>
+      <c r="X194" s="1">
+        <v>173.36680000000001</v>
+      </c>
+    </row>
+    <row r="195" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I195" s="1">
         <v>283.26</v>
       </c>
@@ -13333,8 +13910,11 @@
       <c r="W195" s="1">
         <v>172.94810000000001</v>
       </c>
-    </row>
-    <row r="196" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X195" s="1">
+        <v>172.94810000000001</v>
+      </c>
+    </row>
+    <row r="196" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I196" s="1">
         <v>283.16000000000003</v>
       </c>
@@ -13377,8 +13957,11 @@
       <c r="W196" s="1">
         <v>176.29820000000001</v>
       </c>
-    </row>
-    <row r="197" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X196" s="1">
+        <v>176.29820000000001</v>
+      </c>
+    </row>
+    <row r="197" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I197" s="1">
         <v>283.06</v>
       </c>
@@ -13421,8 +14004,11 @@
       <c r="W197" s="1">
         <v>180.48580000000001</v>
       </c>
-    </row>
-    <row r="198" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X197" s="1">
+        <v>180.48580000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I198" s="1">
         <v>282.95999999999998</v>
       </c>
@@ -13457,16 +14043,19 @@
         <v>181.74199999999999</v>
       </c>
       <c r="U198" s="1">
-        <v>181.74209999999999</v>
+        <v>181.74199999999999</v>
       </c>
       <c r="V198" s="1">
         <v>181.74199999999999</v>
       </c>
       <c r="W198" s="1">
-        <v>181.74209999999999</v>
-      </c>
-    </row>
-    <row r="199" spans="9:23" x14ac:dyDescent="0.45">
+        <v>181.74199999999999</v>
+      </c>
+      <c r="X198" s="1">
+        <v>181.74199999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I199" s="1">
         <v>282.86</v>
       </c>
@@ -13509,8 +14098,11 @@
       <c r="W199" s="1">
         <v>189.6985</v>
       </c>
-    </row>
-    <row r="200" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X199" s="1">
+        <v>189.6985</v>
+      </c>
+    </row>
+    <row r="200" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I200" s="1">
         <v>282.76</v>
       </c>
@@ -13553,8 +14145,11 @@
       <c r="W200" s="1">
         <v>189.27969999999999</v>
       </c>
-    </row>
-    <row r="201" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X200" s="1">
+        <v>189.27969999999999</v>
+      </c>
+    </row>
+    <row r="201" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I201" s="1">
         <v>282.66000000000003</v>
       </c>
@@ -13597,8 +14192,11 @@
       <c r="W201" s="1">
         <v>179.6482</v>
       </c>
-    </row>
-    <row r="202" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X201" s="1">
+        <v>179.6482</v>
+      </c>
+    </row>
+    <row r="202" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I202" s="1">
         <v>282.56</v>
       </c>
@@ -13641,8 +14239,11 @@
       <c r="W202" s="1">
         <v>189.27969999999999</v>
       </c>
-    </row>
-    <row r="203" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X202" s="1">
+        <v>189.27969999999999</v>
+      </c>
+    </row>
+    <row r="203" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I203" s="1">
         <v>282.45999999999998</v>
       </c>
@@ -13685,8 +14286,11 @@
       <c r="W203" s="1">
         <v>182.5796</v>
       </c>
-    </row>
-    <row r="204" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X203" s="1">
+        <v>182.5796</v>
+      </c>
+    </row>
+    <row r="204" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I204" s="1">
         <v>282.36</v>
       </c>
@@ -13729,8 +14333,11 @@
       <c r="W204" s="1">
         <v>186.3484</v>
       </c>
-    </row>
-    <row r="205" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X204" s="1">
+        <v>186.3484</v>
+      </c>
+    </row>
+    <row r="205" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I205" s="1">
         <v>282.26</v>
       </c>
@@ -13773,8 +14380,11 @@
       <c r="W205" s="1">
         <v>181.74199999999999</v>
       </c>
-    </row>
-    <row r="206" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X205" s="1">
+        <v>181.74199999999999</v>
+      </c>
+    </row>
+    <row r="206" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I206" s="1">
         <v>282.16000000000003</v>
       </c>
@@ -13817,8 +14427,11 @@
       <c r="W206" s="1">
         <v>181.32329999999999</v>
       </c>
-    </row>
-    <row r="207" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X206" s="1">
+        <v>181.32329999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I207" s="1">
         <v>282.06</v>
       </c>
@@ -13861,8 +14474,11 @@
       <c r="W207" s="1">
         <v>181.74199999999999</v>
       </c>
-    </row>
-    <row r="208" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X207" s="1">
+        <v>181.74199999999999</v>
+      </c>
+    </row>
+    <row r="208" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I208" s="1">
         <v>281.95999999999998</v>
       </c>
@@ -13905,8 +14521,11 @@
       <c r="W208" s="1">
         <v>185.51089999999999</v>
       </c>
-    </row>
-    <row r="209" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X208" s="1">
+        <v>185.51089999999999</v>
+      </c>
+    </row>
+    <row r="209" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I209" s="1">
         <v>281.86</v>
       </c>
@@ -13949,8 +14568,11 @@
       <c r="W209" s="1">
         <v>171.273</v>
       </c>
-    </row>
-    <row r="210" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X209" s="1">
+        <v>171.273</v>
+      </c>
+    </row>
+    <row r="210" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I210" s="1">
         <v>281.76</v>
       </c>
@@ -13993,8 +14615,11 @@
       <c r="W210" s="1">
         <v>182.9983</v>
       </c>
-    </row>
-    <row r="211" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X210" s="1">
+        <v>182.9983</v>
+      </c>
+    </row>
+    <row r="211" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I211" s="1">
         <v>281.66000000000003</v>
       </c>
@@ -14037,8 +14662,11 @@
       <c r="W211" s="1">
         <v>184.25460000000001</v>
       </c>
-    </row>
-    <row r="212" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X211" s="1">
+        <v>184.25460000000001</v>
+      </c>
+    </row>
+    <row r="212" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I212" s="1">
         <v>281.56</v>
       </c>
@@ -14081,8 +14709,11 @@
       <c r="W212" s="1">
         <v>174.20439999999999</v>
       </c>
-    </row>
-    <row r="213" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X212" s="1">
+        <v>174.20439999999999</v>
+      </c>
+    </row>
+    <row r="213" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I213" s="1">
         <v>281.45999999999998</v>
       </c>
@@ -14125,8 +14756,11 @@
       <c r="W213" s="1">
         <v>172.52930000000001</v>
       </c>
-    </row>
-    <row r="214" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X213" s="1">
+        <v>172.52930000000001</v>
+      </c>
+    </row>
+    <row r="214" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I214" s="1">
         <v>281.36</v>
       </c>
@@ -14169,8 +14803,11 @@
       <c r="W214" s="1">
         <v>161.64150000000001</v>
       </c>
-    </row>
-    <row r="215" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X214" s="1">
+        <v>161.64150000000001</v>
+      </c>
+    </row>
+    <row r="215" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I215" s="1">
         <v>281.26</v>
       </c>
@@ -14213,8 +14850,11 @@
       <c r="W215" s="1">
         <v>169.17920000000001</v>
       </c>
-    </row>
-    <row r="216" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X215" s="1">
+        <v>169.17920000000001</v>
+      </c>
+    </row>
+    <row r="216" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I216" s="1">
         <v>281.16000000000003</v>
       </c>
@@ -14257,8 +14897,11 @@
       <c r="W216" s="1">
         <v>165.41040000000001</v>
       </c>
-    </row>
-    <row r="217" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X216" s="1">
+        <v>165.41040000000001</v>
+      </c>
+    </row>
+    <row r="217" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I217" s="1">
         <v>281.06</v>
       </c>
@@ -14301,8 +14944,11 @@
       <c r="W217" s="1">
         <v>178.392</v>
       </c>
-    </row>
-    <row r="218" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X217" s="1">
+        <v>178.392</v>
+      </c>
+    </row>
+    <row r="218" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I218" s="1">
         <v>280.95999999999998</v>
       </c>
@@ -14345,8 +14991,11 @@
       <c r="W218" s="1">
         <v>167.9229</v>
       </c>
-    </row>
-    <row r="219" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X218" s="1">
+        <v>167.9229</v>
+      </c>
+    </row>
+    <row r="219" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I219" s="1">
         <v>280.86</v>
       </c>
@@ -14389,8 +15038,11 @@
       <c r="W219" s="1">
         <v>167.5042</v>
       </c>
-    </row>
-    <row r="220" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X219" s="1">
+        <v>167.5042</v>
+      </c>
+    </row>
+    <row r="220" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I220" s="1">
         <v>280.76</v>
       </c>
@@ -14433,8 +15085,11 @@
       <c r="W220" s="1">
         <v>160.3853</v>
       </c>
-    </row>
-    <row r="221" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X220" s="1">
+        <v>160.3853</v>
+      </c>
+    </row>
+    <row r="221" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I221" s="1">
         <v>280.66000000000003</v>
       </c>
@@ -14477,8 +15132,11 @@
       <c r="W221" s="1">
         <v>190.95480000000001</v>
       </c>
-    </row>
-    <row r="222" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X221" s="1">
+        <v>190.95480000000001</v>
+      </c>
+    </row>
+    <row r="222" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I222" s="1">
         <v>280.56</v>
       </c>
@@ -14521,8 +15179,11 @@
       <c r="W222" s="1">
         <v>176.29820000000001</v>
       </c>
-    </row>
-    <row r="223" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X222" s="1">
+        <v>176.29820000000001</v>
+      </c>
+    </row>
+    <row r="223" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I223" s="1">
         <v>280.45999999999998</v>
       </c>
@@ -14565,8 +15226,11 @@
       <c r="W223" s="1">
         <v>175.8794</v>
       </c>
-    </row>
-    <row r="224" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X223" s="1">
+        <v>175.8794</v>
+      </c>
+    </row>
+    <row r="224" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I224" s="1">
         <v>280.36</v>
       </c>
@@ -14609,8 +15273,11 @@
       <c r="W224" s="1">
         <v>163.7353</v>
       </c>
-    </row>
-    <row r="225" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X224" s="1">
+        <v>163.7353</v>
+      </c>
+    </row>
+    <row r="225" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I225" s="1">
         <v>280.26</v>
       </c>
@@ -14653,8 +15320,11 @@
       <c r="W225" s="1">
         <v>183.4171</v>
       </c>
-    </row>
-    <row r="226" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X225" s="1">
+        <v>183.4171</v>
+      </c>
+    </row>
+    <row r="226" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I226" s="1">
         <v>280.16000000000003</v>
       </c>
@@ -14697,8 +15367,11 @@
       <c r="W226" s="1">
         <v>175.4606</v>
       </c>
-    </row>
-    <row r="227" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X226" s="1">
+        <v>175.4606</v>
+      </c>
+    </row>
+    <row r="227" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I227" s="1">
         <v>280.06</v>
       </c>
@@ -14741,8 +15414,11 @@
       <c r="W227" s="1">
         <v>172.94810000000001</v>
       </c>
-    </row>
-    <row r="228" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X227" s="1">
+        <v>172.94810000000001</v>
+      </c>
+    </row>
+    <row r="228" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I228" s="1">
         <v>279.95999999999998</v>
       </c>
@@ -14785,8 +15461,11 @@
       <c r="W228" s="1">
         <v>175.0419</v>
       </c>
-    </row>
-    <row r="229" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X228" s="1">
+        <v>175.0419</v>
+      </c>
+    </row>
+    <row r="229" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I229" s="1">
         <v>279.86</v>
       </c>
@@ -14829,8 +15508,11 @@
       <c r="W229" s="1">
         <v>180.06700000000001</v>
       </c>
-    </row>
-    <row r="230" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X229" s="1">
+        <v>180.06700000000001</v>
+      </c>
+    </row>
+    <row r="230" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I230" s="1">
         <v>279.76</v>
       </c>
@@ -14873,8 +15555,11 @@
       <c r="W230" s="1">
         <v>170.43549999999999</v>
       </c>
-    </row>
-    <row r="231" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X230" s="1">
+        <v>170.43549999999999</v>
+      </c>
+    </row>
+    <row r="231" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I231" s="1">
         <v>279.66000000000003</v>
       </c>
@@ -14917,8 +15602,11 @@
       <c r="W231" s="1">
         <v>191.37350000000001</v>
       </c>
-    </row>
-    <row r="232" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X231" s="1">
+        <v>191.37350000000001</v>
+      </c>
+    </row>
+    <row r="232" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I232" s="1">
         <v>279.56</v>
       </c>
@@ -14961,8 +15649,11 @@
       <c r="W232" s="1">
         <v>172.52930000000001</v>
       </c>
-    </row>
-    <row r="233" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X232" s="1">
+        <v>172.52930000000001</v>
+      </c>
+    </row>
+    <row r="233" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I233" s="1">
         <v>279.45999999999998</v>
       </c>
@@ -15005,8 +15696,11 @@
       <c r="W233" s="1">
         <v>177.97319999999999</v>
       </c>
-    </row>
-    <row r="234" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X233" s="1">
+        <v>177.97319999999999</v>
+      </c>
+    </row>
+    <row r="234" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I234" s="1">
         <v>279.36</v>
       </c>
@@ -15049,8 +15743,11 @@
       <c r="W234" s="1">
         <v>176.29820000000001</v>
       </c>
-    </row>
-    <row r="235" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X234" s="1">
+        <v>176.29820000000001</v>
+      </c>
+    </row>
+    <row r="235" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I235" s="1">
         <v>279.26</v>
       </c>
@@ -15093,8 +15790,11 @@
       <c r="W235" s="1">
         <v>189.6985</v>
       </c>
-    </row>
-    <row r="236" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X235" s="1">
+        <v>189.6985</v>
+      </c>
+    </row>
+    <row r="236" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I236" s="1">
         <v>279.16000000000003</v>
       </c>
@@ -15137,8 +15837,11 @@
       <c r="W236" s="1">
         <v>162.47909999999999</v>
       </c>
-    </row>
-    <row r="237" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X236" s="1">
+        <v>162.47909999999999</v>
+      </c>
+    </row>
+    <row r="237" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I237" s="1">
         <v>279.06</v>
       </c>
@@ -15181,8 +15884,11 @@
       <c r="W237" s="1">
         <v>157.0352</v>
       </c>
-    </row>
-    <row r="238" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X237" s="1">
+        <v>157.0352</v>
+      </c>
+    </row>
+    <row r="238" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I238" s="1">
         <v>278.95999999999998</v>
       </c>
@@ -15225,8 +15931,11 @@
       <c r="W238" s="1">
         <v>177.13570000000001</v>
       </c>
-    </row>
-    <row r="239" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X238" s="1">
+        <v>177.13570000000001</v>
+      </c>
+    </row>
+    <row r="239" spans="9:24" x14ac:dyDescent="0.45">
       <c r="I239" s="1">
         <v>278.86</v>
       </c>
@@ -15269,8 +15978,11 @@
       <c r="W239" s="1">
         <v>178.392</v>
       </c>
-    </row>
-    <row r="240" spans="9:23" x14ac:dyDescent="0.45">
+      <c r="X239" s="1">
+        <v>178.392</v>
+      </c>
+    </row>
+    <row r="240" spans="9:24" x14ac:dyDescent="0.45">
       <c r="S240" s="1">
         <v>64.760000000000005</v>
       </c>
@@ -15286,8 +15998,11 @@
       <c r="W240" s="1">
         <v>174.62309999999999</v>
       </c>
-    </row>
-    <row r="241" spans="19:23" x14ac:dyDescent="0.45">
+      <c r="X240" s="1">
+        <v>174.62309999999999</v>
+      </c>
+    </row>
+    <row r="241" spans="19:24" x14ac:dyDescent="0.45">
       <c r="S241" s="1">
         <v>64.66</v>
       </c>
@@ -15303,8 +16018,11 @@
       <c r="W241" s="1">
         <v>172.11060000000001</v>
       </c>
-    </row>
-    <row r="242" spans="19:23" x14ac:dyDescent="0.45">
+      <c r="X241" s="1">
+        <v>172.11060000000001</v>
+      </c>
+    </row>
+    <row r="242" spans="19:24" x14ac:dyDescent="0.45">
       <c r="S242" s="1">
         <v>64.56</v>
       </c>
@@ -15320,8 +16038,11 @@
       <c r="W242" s="1">
         <v>164.1541</v>
       </c>
-    </row>
-    <row r="243" spans="19:23" x14ac:dyDescent="0.45">
+      <c r="X242" s="1">
+        <v>164.1541</v>
+      </c>
+    </row>
+    <row r="243" spans="19:24" x14ac:dyDescent="0.45">
       <c r="S243" s="1">
         <v>64.459999999999994</v>
       </c>
@@ -15337,8 +16058,11 @@
       <c r="W243" s="1">
         <v>175.0419</v>
       </c>
-    </row>
-    <row r="244" spans="19:23" x14ac:dyDescent="0.45">
+      <c r="X243" s="1">
+        <v>175.0419</v>
+      </c>
+    </row>
+    <row r="244" spans="19:24" x14ac:dyDescent="0.45">
       <c r="S244" s="1">
         <v>64.36</v>
       </c>
@@ -15354,8 +16078,11 @@
       <c r="W244" s="1">
         <v>178.8107</v>
       </c>
-    </row>
-    <row r="245" spans="19:23" x14ac:dyDescent="0.45">
+      <c r="X244" s="1">
+        <v>178.8107</v>
+      </c>
+    </row>
+    <row r="245" spans="19:24" x14ac:dyDescent="0.45">
       <c r="S245" s="1">
         <v>64.260000000000005</v>
       </c>
@@ -15371,8 +16098,11 @@
       <c r="W245" s="1">
         <v>188.02350000000001</v>
       </c>
-    </row>
-    <row r="246" spans="19:23" x14ac:dyDescent="0.45">
+      <c r="X245" s="1">
+        <v>188.02350000000001</v>
+      </c>
+    </row>
+    <row r="246" spans="19:24" x14ac:dyDescent="0.45">
       <c r="S246" s="1">
         <v>64.16</v>
       </c>
@@ -15388,8 +16118,11 @@
       <c r="W246" s="1">
         <v>179.6482</v>
       </c>
-    </row>
-    <row r="247" spans="19:23" x14ac:dyDescent="0.45">
+      <c r="X246" s="1">
+        <v>179.6482</v>
+      </c>
+    </row>
+    <row r="247" spans="19:24" x14ac:dyDescent="0.45">
       <c r="S247" s="1">
         <v>64.06</v>
       </c>
@@ -15405,8 +16138,11 @@
       <c r="W247" s="1">
         <v>178.392</v>
       </c>
-    </row>
-    <row r="248" spans="19:23" x14ac:dyDescent="0.45">
+      <c r="X247" s="1">
+        <v>178.392</v>
+      </c>
+    </row>
+    <row r="248" spans="19:24" x14ac:dyDescent="0.45">
       <c r="S248" s="1">
         <v>63.96</v>
       </c>
@@ -15420,6 +16156,9 @@
         <v>171.6918</v>
       </c>
       <c r="W248" s="1">
+        <v>171.6918</v>
+      </c>
+      <c r="X248" s="1">
         <v>171.6918</v>
       </c>
     </row>

</xml_diff>